<commit_message>
updated prints statements to include logging
</commit_message>
<xml_diff>
--- a/autoast/4_jobs_Sunny.xlsx
+++ b/autoast/4_jobs_Sunny.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\SharedWork\Northeast_WMU_Bulk_status\AST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\GitHubAutoAST\gss_authorizations\autoast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F933E01-633C-4198-8689-70D3DE4787EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28935" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="Shapefile Info" sheetId="1" r:id="rId1"/>
+    <sheet name="ast_config" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -130,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,31 +473,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="105.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="111.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="105.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="111.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -574,7 +573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -606,7 +605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -638,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -670,7 +669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -702,7 +701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -734,7 +733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -766,7 +765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -798,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -832,15 +831,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{2255374A-3274-4A6A-AF1D-3156F1A400B8}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{F4B204E4-7081-4402-A922-2044EAEAEB47}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{05D61C25-3DD0-4001-8BE6-7830CB26D838}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{5D5C1EFB-E836-4697-969E-329071772BB1}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{9B7D5943-AB42-488A-B8CB-ECAB4139B2FE}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{7DFD5AF7-EC70-437D-A91E-31B7F6413897}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{3A3FFB68-8907-4F6E-9642-B66957C22205}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{66AD62CF-9E34-47E1-BEC5-2D430850AFBE}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{DCED0DE5-FDE0-4CF4-B3DA-9D47F3971ECA}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>